<commit_message>
Added function to allow changing df in excel
</commit_message>
<xml_diff>
--- a/src/Data/DataFrames/setup/setup.xlsx
+++ b/src/Data/DataFrames/setup/setup.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,84 +369,68 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>datnumplus</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>datetime</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>datnumplus</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>i_sense</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FastScan</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>FastScanCh0</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>FastScanCh1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>FastScanCh2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>FastScanCh3</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>fd0adc</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>fd1adc</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>fd2adc</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>fd3adc</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Wednesday, January 1, 2020 00:00:00</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Changes to data fiels
Might want to stop saving so many backups....
</commit_message>
<xml_diff>
--- a/src/Data/DataFrames/setup/setup.xlsx
+++ b/src/Data/DataFrames/setup/setup.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,37 +379,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>x_array</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>y_array</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>i_sense</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>FastScan</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>FastScanCh0</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>FastScanCh1</t>
+          <t>entx</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>FastScanCh2</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>FastScanCh3</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Junk</t>
+          <t>enty</t>
         </is>
       </c>
     </row>
@@ -427,25 +417,6 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>